<commit_message>
no sound yet for some reason...
for some reason it's just straight disconnecting the ym2151 and speech at williams2... have to look into that later when i get more time...
</commit_message>
<xml_diff>
--- a/doc/rom_calc_joust2 - cvsd.xlsx
+++ b/doc/rom_calc_joust2 - cvsd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcoleman\Documents\GitHub\Arcade-Joust2_MiSTer\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aberu\OneDrive\Documents\GitHub\Arcade-Joust2_MiSTer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076CFC16-281F-4390-8479-56FE9086A97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C894F4A-92AA-4076-852B-1541676AC1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14550" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROM Map" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="107">
   <si>
     <t>MAME</t>
   </si>
@@ -317,6 +317,42 @@
   </si>
   <si>
     <t>0010</t>
+  </si>
+  <si>
+    <t>18:14</t>
+  </si>
+  <si>
+    <t>18:13</t>
+  </si>
+  <si>
+    <t>18:12</t>
+  </si>
+  <si>
+    <t>01110</t>
+  </si>
+  <si>
+    <t>01111</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>d'End</t>
+  </si>
+  <si>
+    <t>18:9</t>
+  </si>
+  <si>
+    <t>100010</t>
+  </si>
+  <si>
+    <t>100011</t>
+  </si>
+  <si>
+    <t>1001000</t>
+  </si>
+  <si>
+    <t>1001001000</t>
   </si>
 </sst>
 </file>
@@ -728,7 +764,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -766,7 +802,7 @@
         <v>78</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>79</v>
@@ -1681,7 +1717,7 @@
         <v>66</v>
       </c>
       <c r="E22" s="15">
-        <v>8192</v>
+        <v>16384</v>
       </c>
       <c r="F22" s="15">
         <f t="shared" si="0"/>
@@ -1689,7 +1725,7 @@
       </c>
       <c r="G22" s="15">
         <f t="shared" si="1"/>
-        <v>237567</v>
+        <v>245759</v>
       </c>
       <c r="H22" s="23" t="str">
         <f t="shared" si="3"/>
@@ -1697,18 +1733,22 @@
       </c>
       <c r="I22" s="24" t="str">
         <f t="shared" si="4"/>
-        <v>39FFF</v>
+        <v>3BFFF</v>
       </c>
       <c r="J22" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>000000111001111111111111</v>
+        <v>000000111011111111111111</v>
       </c>
       <c r="K22" s="17" t="str">
         <f t="shared" si="2"/>
         <v>000000111000000000000000</v>
       </c>
-      <c r="L22" s="18"/>
-      <c r="M22" s="19"/>
+      <c r="L22" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
@@ -1724,34 +1764,38 @@
         <v>67</v>
       </c>
       <c r="E23" s="15">
-        <v>8192</v>
+        <v>16384</v>
       </c>
       <c r="F23" s="15">
         <f t="shared" si="0"/>
-        <v>237568</v>
+        <v>245760</v>
       </c>
       <c r="G23" s="15">
         <f t="shared" si="1"/>
-        <v>245759</v>
+        <v>262143</v>
       </c>
       <c r="H23" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>3A000</v>
+        <v>3C000</v>
       </c>
       <c r="I23" s="24" t="str">
         <f t="shared" si="4"/>
-        <v>3BFFF</v>
+        <v>3FFFF</v>
       </c>
       <c r="J23" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>000000111011111111111111</v>
+        <v>000000111111111111111111</v>
       </c>
       <c r="K23" s="17" t="str">
         <f t="shared" si="2"/>
-        <v>000000111010000000000000</v>
-      </c>
-      <c r="L23" s="18"/>
-      <c r="M23" s="19"/>
+        <v>000000111100000000000000</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="M23" s="19" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
@@ -1767,34 +1811,38 @@
         <v>68</v>
       </c>
       <c r="E24" s="15">
-        <v>8192</v>
+        <v>16384</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="0"/>
-        <v>245760</v>
+        <v>262144</v>
       </c>
       <c r="G24" s="15">
         <f t="shared" si="1"/>
-        <v>253951</v>
+        <v>278527</v>
       </c>
       <c r="H24" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>3C000</v>
+        <v>40000</v>
       </c>
       <c r="I24" s="24" t="str">
         <f t="shared" si="4"/>
-        <v>3DFFF</v>
+        <v>43FFF</v>
       </c>
       <c r="J24" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>000000111101111111111111</v>
+        <v>000001000011111111111111</v>
       </c>
       <c r="K24" s="17" t="str">
         <f t="shared" si="2"/>
-        <v>000000111100000000000000</v>
-      </c>
-      <c r="L24" s="18"/>
-      <c r="M24" s="19"/>
+        <v>000001000000000000000000</v>
+      </c>
+      <c r="L24" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -1814,30 +1862,34 @@
       </c>
       <c r="F25" s="15">
         <f t="shared" si="0"/>
-        <v>253952</v>
+        <v>278528</v>
       </c>
       <c r="G25" s="15">
         <f t="shared" si="1"/>
-        <v>258047</v>
+        <v>282623</v>
       </c>
       <c r="H25" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>3E000</v>
+        <v>44000</v>
       </c>
       <c r="I25" s="24" t="str">
         <f t="shared" si="4"/>
-        <v>3EFFF</v>
+        <v>44FFF</v>
       </c>
       <c r="J25" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>000000111110111111111111</v>
+        <v>000001000100111111111111</v>
       </c>
       <c r="K25" s="17" t="str">
         <f t="shared" si="2"/>
-        <v>000000111110000000000000</v>
-      </c>
-      <c r="L25" s="18"/>
-      <c r="M25" s="19"/>
+        <v>000001000100000000000000</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="M25" s="19" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
@@ -1855,30 +1907,34 @@
       </c>
       <c r="F26" s="15">
         <f t="shared" si="0"/>
-        <v>258048</v>
+        <v>282624</v>
       </c>
       <c r="G26" s="15">
         <f t="shared" si="1"/>
-        <v>262143</v>
+        <v>286719</v>
       </c>
       <c r="H26" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>3F000</v>
+        <v>45000</v>
       </c>
       <c r="I26" s="24" t="str">
         <f t="shared" si="4"/>
-        <v>3FFFF</v>
+        <v>45FFF</v>
       </c>
       <c r="J26" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>000000111111111111111111</v>
+        <v>000001000101111111111111</v>
       </c>
       <c r="K26" s="17" t="str">
         <f t="shared" si="2"/>
-        <v>000000111111000000000000</v>
-      </c>
-      <c r="L26" s="18"/>
-      <c r="M26" s="19"/>
+        <v>000001000101000000000000</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="M26" s="19" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -1898,30 +1954,34 @@
       </c>
       <c r="F27" s="15">
         <f t="shared" si="0"/>
-        <v>262144</v>
+        <v>286720</v>
       </c>
       <c r="G27" s="15">
         <f t="shared" si="1"/>
-        <v>270335</v>
+        <v>294911</v>
       </c>
       <c r="H27" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>40000</v>
+        <v>46000</v>
       </c>
       <c r="I27" s="24" t="str">
         <f t="shared" si="4"/>
-        <v>41FFF</v>
+        <v>47FFF</v>
       </c>
       <c r="J27" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>000001000001111111111111</v>
+        <v>000001000111111111111111</v>
       </c>
       <c r="K27" s="17" t="str">
         <f t="shared" si="2"/>
-        <v>000001000000000000000000</v>
-      </c>
-      <c r="L27" s="18"/>
-      <c r="M27" s="19"/>
+        <v>000001000110000000000000</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="M27" s="19" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -1941,30 +2001,34 @@
       </c>
       <c r="F28" s="15">
         <f t="shared" si="0"/>
-        <v>270336</v>
+        <v>294912</v>
       </c>
       <c r="G28" s="15">
         <f t="shared" si="1"/>
-        <v>274431</v>
+        <v>299007</v>
       </c>
       <c r="H28" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>42000</v>
+        <v>48000</v>
       </c>
       <c r="I28" s="24" t="str">
         <f t="shared" si="4"/>
-        <v>42FFF</v>
+        <v>48FFF</v>
       </c>
       <c r="J28" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>000001000010111111111111</v>
+        <v>000001001000111111111111</v>
       </c>
       <c r="K28" s="17" t="str">
         <f t="shared" si="2"/>
-        <v>000001000010000000000000</v>
-      </c>
-      <c r="L28" s="18"/>
-      <c r="M28" s="19"/>
+        <v>000001001000000000000000</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="M28" s="19" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
@@ -1984,30 +2048,34 @@
       </c>
       <c r="F29" s="15">
         <f t="shared" si="0"/>
-        <v>274432</v>
+        <v>299008</v>
       </c>
       <c r="G29" s="15">
         <f t="shared" si="1"/>
-        <v>274943</v>
+        <v>299519</v>
       </c>
       <c r="H29" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>43000</v>
+        <v>49000</v>
       </c>
       <c r="I29" s="24" t="str">
         <f t="shared" si="4"/>
-        <v>431FF</v>
+        <v>491FF</v>
       </c>
       <c r="J29" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>000001000011000111111111</v>
+        <v>000001001001000111111111</v>
       </c>
       <c r="K29" s="17" t="str">
         <f t="shared" si="2"/>
-        <v>000001000011000000000000</v>
-      </c>
-      <c r="L29" s="18"/>
-      <c r="M29" s="19"/>
+        <v>000001001001000000000000</v>
+      </c>
+      <c r="L29" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="M29" s="19" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
@@ -2018,10 +2086,10 @@
     <cfRule type="duplicateValues" dxfId="2" priority="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J29">
-    <cfRule type="duplicateValues" dxfId="1" priority="102"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="118"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K29">
-    <cfRule type="duplicateValues" dxfId="0" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="120"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>